<commit_message>
première partie session 06
</commit_message>
<xml_diff>
--- a/slides/Plan concepts.xlsx
+++ b/slides/Plan concepts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/196f0b5afced95ca/Dev/Python/cours-deeplearning-2020/slides/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="966" documentId="8_{54925A65-0A31-4BBD-84F6-D26AACE90504}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F893205D-0959-461A-8881-A56FE294BF00}"/>
+  <xr:revisionPtr revIDLastSave="1066" documentId="8_{54925A65-0A31-4BBD-84F6-D26AACE90504}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{CA02772A-163F-4767-8622-3BD3C630E581}"/>
   <bookViews>
-    <workbookView xWindow="24165" yWindow="1995" windowWidth="7500" windowHeight="6000" xr2:uid="{931F91DC-39E4-49EC-BA01-FB85E43D97B9}"/>
+    <workbookView xWindow="-11625" yWindow="5355" windowWidth="21600" windowHeight="11385" xr2:uid="{931F91DC-39E4-49EC-BA01-FB85E43D97B9}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="103">
   <si>
     <t>Notebook</t>
   </si>
@@ -231,6 +231,117 @@
   </si>
   <si>
     <t>Training a state of the art model</t>
+  </si>
+  <si>
+    <t>Imagenette dataset as a proxy</t>
+  </si>
+  <si>
+    <t>Normalization</t>
+  </si>
+  <si>
+    <t>… important for pretrained models</t>
+  </si>
+  <si>
+    <t>Progressive resizing</t>
+  </si>
+  <si>
+    <t>… another form of data augmentation</t>
+  </si>
+  <si>
+    <t>Test time augmentation</t>
+  </si>
+  <si>
+    <t>Mixup</t>
+  </si>
+  <si>
+    <t>Label Smoothing</t>
+  </si>
+  <si>
+    <t>… important to iterate quickly</t>
+  </si>
+  <si>
+    <t>… need to train more epochs</t>
+  </si>
+  <si>
+    <t>… inference much slower</t>
+  </si>
+  <si>
+    <t>08_collab</t>
+  </si>
+  <si>
+    <t>Collaborative filtering deep dive</t>
+  </si>
+  <si>
+    <t>MovieLens</t>
+  </si>
+  <si>
+    <t>Latent factors</t>
+  </si>
+  <si>
+    <t>Embedding layer</t>
+  </si>
+  <si>
+    <t>… learn a numeric representation</t>
+  </si>
+  <si>
+    <t>Class, __init__</t>
+  </si>
+  <si>
+    <t>DotProduct module</t>
+  </si>
+  <si>
+    <t>Add bias</t>
+  </si>
+  <si>
+    <t>Overfitting</t>
+  </si>
+  <si>
+    <t>Weight decay = L2 regularization</t>
+  </si>
+  <si>
+    <t>Create Embedding module</t>
+  </si>
+  <si>
+    <t>nn.Parameter</t>
+  </si>
+  <si>
+    <t>nn.Module</t>
+  </si>
+  <si>
+    <t>Interpreting embeddings</t>
+  </si>
+  <si>
+    <t>Principal Component Analysis</t>
+  </si>
+  <si>
+    <t>fastai.collab</t>
+  </si>
+  <si>
+    <t>collab_learner</t>
+  </si>
+  <si>
+    <t>Embedding distance</t>
+  </si>
+  <si>
+    <t>nn.CosineSimilarity</t>
+  </si>
+  <si>
+    <t>Bootstrapping a collab model</t>
+  </si>
+  <si>
+    <t>risks you need to plan for</t>
+  </si>
+  <si>
+    <t>Deep learning for collaborative filtering</t>
+  </si>
+  <si>
+    <t>embedding size : get_emb_sz</t>
+  </si>
+  <si>
+    <t>use_nn=True : CollabNN</t>
+  </si>
+  <si>
+    <t>kwargs and delegates</t>
   </si>
 </sst>
 </file>
@@ -287,11 +398,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -606,10 +721,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C51D786-F23B-454D-8D07-91BA6BA38ED0}">
-  <dimension ref="A1:E73"/>
+  <dimension ref="A1:H78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="103" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="D2" zoomScale="103" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -619,9 +734,10 @@
     <col min="3" max="3" width="16" customWidth="1"/>
     <col min="4" max="4" width="21.42578125" customWidth="1"/>
     <col min="5" max="5" width="28.140625" customWidth="1"/>
+    <col min="7" max="8" width="24.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -634,8 +750,14 @@
       <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -643,13 +765,19 @@
         <v>31</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>64</v>
+        <v>29</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -657,480 +785,687 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="E4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" t="s">
+        <v>77</v>
+      </c>
+      <c r="H4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" t="s">
+        <v>77</v>
+      </c>
+      <c r="H5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>77</v>
+      </c>
+      <c r="H6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" t="s">
+        <v>77</v>
+      </c>
+      <c r="H7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>2</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" t="s">
+        <v>77</v>
+      </c>
+      <c r="H8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>2</v>
       </c>
       <c r="B9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" t="s">
+        <v>77</v>
+      </c>
+      <c r="H9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>2</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" t="s">
+        <v>37</v>
+      </c>
+      <c r="G10" t="s">
+        <v>77</v>
+      </c>
+      <c r="H10" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" t="s">
+        <v>41</v>
+      </c>
+      <c r="G11" t="s">
+        <v>77</v>
+      </c>
+      <c r="H11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>2</v>
       </c>
       <c r="B12" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" t="s">
+        <v>38</v>
+      </c>
+      <c r="G12" t="s">
+        <v>77</v>
+      </c>
+      <c r="H12" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>2</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" t="s">
+        <v>39</v>
+      </c>
+      <c r="G13" t="s">
+        <v>77</v>
+      </c>
+      <c r="H13" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>2</v>
       </c>
       <c r="B14" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" t="s">
+        <v>40</v>
+      </c>
+      <c r="G14" t="s">
+        <v>77</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>2</v>
       </c>
       <c r="B15" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" t="s">
+        <v>43</v>
+      </c>
+      <c r="G15" t="s">
+        <v>77</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>2</v>
       </c>
       <c r="B16" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="G16" t="s">
+        <v>77</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>2</v>
       </c>
       <c r="B17" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" t="s">
+        <v>44</v>
+      </c>
+      <c r="G17" t="s">
+        <v>77</v>
+      </c>
+      <c r="H17" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>2</v>
       </c>
       <c r="B18" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>29</v>
+      </c>
+      <c r="E18" t="s">
+        <v>45</v>
+      </c>
+      <c r="G18" t="s">
+        <v>77</v>
+      </c>
+      <c r="H18" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>2</v>
       </c>
       <c r="B19" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>29</v>
+      </c>
+      <c r="E19" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>29</v>
+      </c>
+      <c r="E20" t="s">
+        <v>47</v>
+      </c>
+      <c r="G20" t="s">
+        <v>77</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B21" s="3"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>29</v>
+      </c>
+      <c r="E21" t="s">
+        <v>48</v>
+      </c>
+      <c r="G21" t="s">
+        <v>77</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>2</v>
       </c>
       <c r="B22" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>29</v>
+      </c>
+      <c r="E22" t="s">
+        <v>49</v>
+      </c>
+      <c r="G22" t="s">
+        <v>77</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>2</v>
       </c>
       <c r="B23" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>29</v>
+      </c>
+      <c r="E23" t="s">
+        <v>50</v>
+      </c>
+      <c r="G23" t="s">
+        <v>77</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>2</v>
       </c>
       <c r="B24" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>29</v>
+      </c>
+      <c r="E24" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>2</v>
       </c>
       <c r="B25" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>29</v>
+      </c>
+      <c r="E25" t="s">
+        <v>52</v>
+      </c>
+      <c r="G25" t="s">
+        <v>77</v>
+      </c>
+      <c r="H25" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G26" t="s">
+        <v>77</v>
+      </c>
+      <c r="H26" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>2</v>
       </c>
       <c r="B27" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D27" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>2</v>
       </c>
       <c r="B28" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="G28" t="s">
+        <v>77</v>
+      </c>
+      <c r="H28" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>2</v>
       </c>
       <c r="B29" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D29" t="s">
+        <v>29</v>
+      </c>
+      <c r="E29" t="s">
+        <v>54</v>
+      </c>
+      <c r="G29" t="s">
+        <v>77</v>
+      </c>
+      <c r="H29" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>2</v>
       </c>
       <c r="B30" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D30" t="s">
+        <v>29</v>
+      </c>
+      <c r="E30" t="s">
+        <v>57</v>
+      </c>
+      <c r="G30" t="s">
+        <v>77</v>
+      </c>
+      <c r="H30" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>2</v>
       </c>
       <c r="B31" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
+        <v>29</v>
+      </c>
+      <c r="E31" t="s">
+        <v>55</v>
+      </c>
+      <c r="G31" t="s">
+        <v>77</v>
+      </c>
+      <c r="H31" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>2</v>
       </c>
       <c r="B32" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
+        <v>29</v>
+      </c>
+      <c r="E32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>2</v>
       </c>
       <c r="B33" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>29</v>
-      </c>
-      <c r="B37" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>29</v>
-      </c>
-      <c r="B38" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>29</v>
-      </c>
-      <c r="B40" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>29</v>
-      </c>
-      <c r="B41" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>29</v>
-      </c>
-      <c r="B42" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>29</v>
-      </c>
-      <c r="B43" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>29</v>
-      </c>
-      <c r="B44" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>29</v>
-      </c>
-      <c r="B45" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>29</v>
-      </c>
-      <c r="B46" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>29</v>
-      </c>
-      <c r="B47" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>29</v>
-      </c>
-      <c r="B48" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>29</v>
-      </c>
-      <c r="B50" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>29</v>
-      </c>
-      <c r="B51" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>29</v>
-      </c>
-      <c r="B52" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>29</v>
-      </c>
-      <c r="B53" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>29</v>
-      </c>
-      <c r="B54" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>29</v>
-      </c>
-      <c r="B55" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>29</v>
-      </c>
-      <c r="B56" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>29</v>
-      </c>
-      <c r="B57" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>29</v>
-      </c>
-      <c r="B58" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>29</v>
-      </c>
-      <c r="B62" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>29</v>
-      </c>
-      <c r="B63" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>29</v>
-      </c>
-      <c r="B64" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>29</v>
-      </c>
-      <c r="B65" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>29</v>
-      </c>
-      <c r="B66" t="s">
+      <c r="D33" t="s">
+        <v>29</v>
+      </c>
+      <c r="E33" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>29</v>
-      </c>
-      <c r="B67" t="s">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
+        <v>29</v>
+      </c>
+      <c r="E34" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>29</v>
-      </c>
-      <c r="B69" t="s">
+    <row r="35" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D35"/>
+      <c r="E35"/>
+      <c r="G35"/>
+      <c r="H35"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D36" t="s">
+        <v>29</v>
+      </c>
+      <c r="E36" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>29</v>
-      </c>
-      <c r="B70" t="s">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D37" t="s">
+        <v>29</v>
+      </c>
+      <c r="E37" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>29</v>
-      </c>
-      <c r="B71" t="s">
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D38" t="s">
+        <v>29</v>
+      </c>
+      <c r="E38" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>29</v>
-      </c>
-      <c r="B72" t="s">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D39" t="s">
+        <v>29</v>
+      </c>
+      <c r="E39" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>29</v>
-      </c>
-      <c r="B73" t="s">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D40" t="s">
+        <v>29</v>
+      </c>
+      <c r="E40" t="s">
         <v>63</v>
       </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D42" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D44" t="s">
+        <v>64</v>
+      </c>
+      <c r="E44" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D45" t="s">
+        <v>64</v>
+      </c>
+      <c r="E45" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D46" t="s">
+        <v>64</v>
+      </c>
+      <c r="E46" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D47" t="s">
+        <v>64</v>
+      </c>
+      <c r="E47" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D48" t="s">
+        <v>64</v>
+      </c>
+      <c r="E48" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="49" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D49" t="s">
+        <v>64</v>
+      </c>
+      <c r="E49" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="50" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D50" t="s">
+        <v>64</v>
+      </c>
+      <c r="E50" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="51" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D51" t="s">
+        <v>64</v>
+      </c>
+      <c r="E51" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="52" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D52" t="s">
+        <v>64</v>
+      </c>
+      <c r="E52" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="53" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D53" t="s">
+        <v>64</v>
+      </c>
+      <c r="E53" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="54" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D54" t="s">
+        <v>64</v>
+      </c>
+      <c r="E54" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="55" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D55" t="s">
+        <v>64</v>
+      </c>
+      <c r="E55" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="78" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D78" s="1"/>
+      <c r="E78" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>